<commit_message>
to clear and finish
</commit_message>
<xml_diff>
--- a/data/processed/Excels/X_test_sel_k4.xlsx
+++ b/data/processed/Excels/X_test_sel_k4.xlsx
@@ -883,7 +883,7 @@
         <v>162</v>
       </c>
       <c r="C32" t="n">
-        <v>53.2</v>
+        <v>50.55</v>
       </c>
       <c r="D32" t="n">
         <v>25</v>
@@ -900,7 +900,7 @@
         <v>38.5</v>
       </c>
       <c r="D33" t="n">
-        <v>67</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="34">
@@ -1261,7 +1261,7 @@
         <v>80</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>13.35</v>
       </c>
       <c r="D59" t="n">
         <v>22</v>
@@ -1751,7 +1751,7 @@
         <v>74</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>13.35</v>
       </c>
       <c r="D94" t="n">
         <v>22</v>
@@ -2031,7 +2031,7 @@
         <v>105</v>
       </c>
       <c r="C114" t="n">
-        <v>0</v>
+        <v>13.35</v>
       </c>
       <c r="D114" t="n">
         <v>24</v>
@@ -2227,7 +2227,7 @@
         <v>115</v>
       </c>
       <c r="C128" t="n">
-        <v>0</v>
+        <v>13.35</v>
       </c>
       <c r="D128" t="n">
         <v>30</v>
@@ -2255,7 +2255,7 @@
         <v>135</v>
       </c>
       <c r="C130" t="n">
-        <v>52.3</v>
+        <v>50.55</v>
       </c>
       <c r="D130" t="n">
         <v>40</v>

</xml_diff>